<commit_message>
small fix + output
</commit_message>
<xml_diff>
--- a/output/portfolio_risk_report.xlsx
+++ b/output/portfolio_risk_report.xlsx
@@ -541,7 +541,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.009623970401021552</v>
+        <v>0.009623969785957349</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -549,7 +549,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.1527757938368975</v>
+        <v>0.152775784073056</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -557,7 +557,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1557.225982230736</v>
+        <v>1557.225456306438</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -573,7 +573,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6964.126305193612</v>
+        <v>6964.123953188649</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -589,7 +589,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-0.1153004051382721</v>
+        <v>-0.1153004051382722</v>
       </c>
     </row>
     <row r="10" spans="1:2">

</xml_diff>